<commit_message>
feat: Add initial Home page component and `evaluaciones.xlsx` data file.
</commit_message>
<xml_diff>
--- a/data/database/evaluaciones.xlsx
+++ b/data/database/evaluaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magod\Documents\Proyectos\Informes PHP\website-ui\data\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AED9914-A815-4EBD-A0B7-6739AF661A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D77F504-EEB2-4ED8-AB5D-578D4F111F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>SIMCE Matemáticas</t>
   </si>
@@ -58,12 +58,36 @@
   </si>
   <si>
     <t>last_run</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>PDF</t>
+  </si>
+  <si>
+    <t>Workflow SIMCE</t>
+  </si>
+  <si>
+    <t>Workflow DIA</t>
+  </si>
+  <si>
+    <t>DIA Extraer respuestas correctas</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>id_evaluation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd\ mmm\ yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,8 +117,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,68 +400,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1">
+        <v>46050</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1">
+        <v>46050</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1">
+        <v>46050</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1">
+        <v>46050</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1">
+        <v>46050</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1">
+        <v>46050</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1">
+        <v>46050</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="1">
+        <v>46050</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1">
+        <v>46050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Implement a FastAPI backend for workflow management and execution, including a new Simce Lenguaje pipeline and an Excel data source.
</commit_message>
<xml_diff>
--- a/data/database/evaluaciones.xlsx
+++ b/data/database/evaluaciones.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Added time into last_run, of workflows list
</commit_message>
<xml_diff>
--- a/data/database/evaluaciones.xlsx
+++ b/data/database/evaluaciones.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -483,8 +479,10 @@
           <t>PDF</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n">
-        <v>46050</v>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2026-01-28 00:00:00</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -506,8 +504,10 @@
           <t>PDF</t>
         </is>
       </c>
-      <c r="E3" s="2" t="n">
-        <v>46050</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2026-01-28 23:18:10</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -529,8 +529,10 @@
           <t>PDF</t>
         </is>
       </c>
-      <c r="E4" s="2" t="n">
-        <v>46050</v>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2026-01-28 00:00:00</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -552,8 +554,10 @@
           <t>PDF</t>
         </is>
       </c>
-      <c r="E5" s="2" t="n">
-        <v>46050</v>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2026-01-28 00:00:00</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -575,8 +579,10 @@
           <t>PDF</t>
         </is>
       </c>
-      <c r="E6" s="2" t="n">
-        <v>46050</v>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2026-01-28 00:00:00</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -598,8 +604,10 @@
           <t>PDF</t>
         </is>
       </c>
-      <c r="E7" s="2" t="n">
-        <v>46050</v>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2026-01-28 00:00:00</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -621,8 +629,10 @@
           <t>PDF</t>
         </is>
       </c>
-      <c r="E8" s="2" t="n">
-        <v>46050</v>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2026-01-28 00:00:00</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -644,8 +654,10 @@
           <t>PDF</t>
         </is>
       </c>
-      <c r="E9" s="2" t="n">
-        <v>46050</v>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2026-01-28 00:00:00</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -667,8 +679,10 @@
           <t>Excel</t>
         </is>
       </c>
-      <c r="E10" s="2" t="n">
-        <v>46050</v>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2026-01-28 00:00:00</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>